<commit_message>
excel added for Mta 2
</commit_message>
<xml_diff>
--- a/Datafile/Protectcsv.xlsx
+++ b/Datafile/Protectcsv.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20295" windowHeight="7950"/>
+    <workbookView windowWidth="20295" windowHeight="7950" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="sheet1" sheetId="1" r:id="rId1"/>
@@ -12,6 +12,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
     <sheet name="Mta1" sheetId="4" r:id="rId4"/>
     <sheet name="PCNewPolicy" sheetId="5" r:id="rId5"/>
+    <sheet name="Mta2propertyType mainresidence " sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
@@ -838,12 +839,19 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="27">
+  <fonts count="28">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -896,6 +904,13 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -903,23 +918,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="18"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -933,26 +941,11 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -964,16 +957,53 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -988,37 +1018,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1032,8 +1032,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1048,7 +1056,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1060,13 +1068,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1084,31 +1116,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1126,7 +1134,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1138,49 +1200,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1192,31 +1212,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1228,7 +1224,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1243,27 +1251,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1295,15 +1292,6 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
       </bottom>
@@ -1325,207 +1313,228 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="15" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="21" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="22" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="24" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="10" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="10" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="58" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" quotePrefix="1">
+    <xf numFmtId="58" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" quotePrefix="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1849,8 +1858,8 @@
   <sheetPr/>
   <dimension ref="A1:CN2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView topLeftCell="BF1" workbookViewId="0">
+      <selection activeCell="BB23" sqref="BB23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="1"/>
@@ -2210,10 +2219,10 @@
       </c>
     </row>
     <row r="2" spans="1:92">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>93</v>
       </c>
       <c r="C2" t="s">
@@ -2267,7 +2276,7 @@
       <c r="S2" t="s">
         <v>107</v>
       </c>
-      <c r="T2" s="2" t="s">
+      <c r="T2" s="3" t="s">
         <v>108</v>
       </c>
       <c r="U2" t="s">
@@ -2276,7 +2285,7 @@
       <c r="V2" t="s">
         <v>110</v>
       </c>
-      <c r="W2" s="2" t="s">
+      <c r="W2" s="3" t="s">
         <v>99</v>
       </c>
       <c r="X2" t="s">
@@ -2288,13 +2297,13 @@
       <c r="Z2" t="s">
         <v>112</v>
       </c>
-      <c r="AA2" s="2" t="s">
+      <c r="AA2" s="3" t="s">
         <v>113</v>
       </c>
       <c r="AB2">
         <v>5</v>
       </c>
-      <c r="AC2" s="2" t="s">
+      <c r="AC2" s="3" t="s">
         <v>114</v>
       </c>
       <c r="AD2" t="s">
@@ -2345,10 +2354,10 @@
       <c r="AS2" t="s">
         <v>126</v>
       </c>
-      <c r="AT2" s="2" t="s">
+      <c r="AT2" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="AU2" s="2" t="s">
+      <c r="AU2" s="3" t="s">
         <v>128</v>
       </c>
       <c r="AV2">
@@ -2426,22 +2435,22 @@
       <c r="BT2">
         <v>25</v>
       </c>
-      <c r="BU2" s="2" t="s">
+      <c r="BU2" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="BV2" s="2" t="s">
+      <c r="BV2" s="3" t="s">
         <v>126</v>
       </c>
       <c r="BW2">
         <v>60</v>
       </c>
-      <c r="BX2" s="2" t="s">
+      <c r="BX2" s="3" t="s">
         <v>127</v>
       </c>
       <c r="BY2">
         <v>90</v>
       </c>
-      <c r="BZ2" s="2" t="s">
+      <c r="BZ2" s="3" t="s">
         <v>125</v>
       </c>
       <c r="CA2">
@@ -2453,22 +2462,22 @@
       <c r="CC2">
         <v>40</v>
       </c>
-      <c r="CD2" s="2" t="s">
+      <c r="CD2" s="3" t="s">
         <v>125</v>
       </c>
       <c r="CE2">
         <v>1</v>
       </c>
-      <c r="CF2" s="2" t="s">
+      <c r="CF2" s="3" t="s">
         <v>128</v>
       </c>
       <c r="CG2">
         <v>0.8</v>
       </c>
-      <c r="CH2" s="2" t="s">
+      <c r="CH2" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="CI2" s="2" t="s">
+      <c r="CI2" s="3" t="s">
         <v>134</v>
       </c>
       <c r="CJ2" t="s">
@@ -2477,7 +2486,7 @@
       <c r="CK2" t="s">
         <v>136</v>
       </c>
-      <c r="CL2" s="2" t="s">
+      <c r="CL2" s="3" t="s">
         <v>137</v>
       </c>
       <c r="CM2">
@@ -2498,271 +2507,271 @@
   <sheetPr/>
   <dimension ref="A1:AR2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="$A1:$XFD1"/>
+    <sheetView topLeftCell="Y1" workbookViewId="0">
+      <selection activeCell="AB5" sqref="AB5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75" outlineLevelRow="1"/>
   <cols>
-    <col min="1" max="1" width="9.14285714285714" style="3"/>
-    <col min="2" max="2" width="28.7142857142857" style="3" customWidth="1"/>
-    <col min="3" max="3" width="13.1428571428571" style="3" customWidth="1"/>
-    <col min="4" max="5" width="9.14285714285714" style="3"/>
-    <col min="6" max="6" width="28" style="3" customWidth="1"/>
-    <col min="7" max="9" width="9.14285714285714" style="3"/>
-    <col min="10" max="10" width="13.8571428571429" style="3" customWidth="1"/>
-    <col min="11" max="11" width="25.2857142857143" style="3" customWidth="1"/>
-    <col min="12" max="12" width="9.14285714285714" style="3"/>
-    <col min="13" max="13" width="14.5714285714286" style="3" customWidth="1"/>
-    <col min="14" max="14" width="9.14285714285714" style="3"/>
-    <col min="15" max="15" width="47.5714285714286" style="3" customWidth="1"/>
-    <col min="16" max="16" width="9.14285714285714" style="3"/>
-    <col min="17" max="17" width="12.2857142857143" style="3" customWidth="1"/>
-    <col min="18" max="18" width="20.7142857142857" style="3" customWidth="1"/>
-    <col min="19" max="19" width="9.14285714285714" style="3"/>
-    <col min="20" max="20" width="12" style="3" customWidth="1"/>
-    <col min="21" max="21" width="9.57142857142857" style="3"/>
-    <col min="22" max="22" width="11.7142857142857" style="3"/>
-    <col min="23" max="23" width="9.14285714285714" style="3"/>
-    <col min="24" max="24" width="23.2857142857143" style="3" customWidth="1"/>
-    <col min="25" max="25" width="34.5714285714286" style="3" customWidth="1"/>
-    <col min="26" max="26" width="23.7142857142857" style="3" customWidth="1"/>
-    <col min="27" max="27" width="43" style="3" customWidth="1"/>
-    <col min="28" max="28" width="10.5714285714286" style="3" customWidth="1"/>
-    <col min="29" max="29" width="9.57142857142857" style="3" customWidth="1"/>
-    <col min="30" max="41" width="9.14285714285714" style="3"/>
-    <col min="42" max="42" width="12.5714285714286" style="3" customWidth="1"/>
-    <col min="43" max="43" width="35.7142857142857" style="3" customWidth="1"/>
-    <col min="44" max="44" width="29.5714285714286" style="3" customWidth="1"/>
-    <col min="45" max="16384" width="9.14285714285714" style="3"/>
+    <col min="1" max="1" width="9.14285714285714" style="4"/>
+    <col min="2" max="2" width="28.7142857142857" style="4" customWidth="1"/>
+    <col min="3" max="3" width="13.1428571428571" style="4" customWidth="1"/>
+    <col min="4" max="5" width="9.14285714285714" style="4"/>
+    <col min="6" max="6" width="28" style="4" customWidth="1"/>
+    <col min="7" max="9" width="9.14285714285714" style="4"/>
+    <col min="10" max="10" width="13.8571428571429" style="4" customWidth="1"/>
+    <col min="11" max="11" width="25.2857142857143" style="4" customWidth="1"/>
+    <col min="12" max="12" width="9.14285714285714" style="4"/>
+    <col min="13" max="13" width="14.5714285714286" style="4" customWidth="1"/>
+    <col min="14" max="14" width="9.14285714285714" style="4"/>
+    <col min="15" max="15" width="47.5714285714286" style="4" customWidth="1"/>
+    <col min="16" max="16" width="9.14285714285714" style="4"/>
+    <col min="17" max="17" width="12.2857142857143" style="4" customWidth="1"/>
+    <col min="18" max="18" width="20.7142857142857" style="4" customWidth="1"/>
+    <col min="19" max="19" width="9.14285714285714" style="4"/>
+    <col min="20" max="20" width="12" style="4" customWidth="1"/>
+    <col min="21" max="21" width="9.57142857142857" style="4"/>
+    <col min="22" max="22" width="11.7142857142857" style="4"/>
+    <col min="23" max="23" width="9.14285714285714" style="4"/>
+    <col min="24" max="24" width="23.2857142857143" style="4" customWidth="1"/>
+    <col min="25" max="25" width="34.5714285714286" style="4" customWidth="1"/>
+    <col min="26" max="26" width="23.7142857142857" style="4" customWidth="1"/>
+    <col min="27" max="27" width="43" style="4" customWidth="1"/>
+    <col min="28" max="28" width="10.5714285714286" style="4" customWidth="1"/>
+    <col min="29" max="29" width="9.57142857142857" style="4" customWidth="1"/>
+    <col min="30" max="41" width="9.14285714285714" style="4"/>
+    <col min="42" max="42" width="12.5714285714286" style="4" customWidth="1"/>
+    <col min="43" max="43" width="35.7142857142857" style="4" customWidth="1"/>
+    <col min="44" max="44" width="29.5714285714286" style="4" customWidth="1"/>
+    <col min="45" max="16384" width="9.14285714285714" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" s="3" customFormat="1" ht="38.25" spans="1:44">
-      <c r="A1" s="3" t="s">
+    <row r="1" s="4" customFormat="1" ht="38.25" spans="1:44">
+      <c r="A1" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="L1" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="M1" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="N1" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="O1" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="P1" s="7" t="s">
         <v>153</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="Q1" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="R1" s="6" t="s">
+      <c r="R1" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="S1" s="6" t="s">
+      <c r="S1" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="T1" s="6" t="s">
+      <c r="T1" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="U1" s="6" t="s">
+      <c r="U1" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="V1" s="6" t="s">
+      <c r="V1" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="W1" s="6" t="s">
+      <c r="W1" s="7" t="s">
         <v>160</v>
       </c>
-      <c r="X1" s="6" t="s">
+      <c r="X1" s="7" t="s">
         <v>161</v>
       </c>
-      <c r="Y1" s="8" t="s">
+      <c r="Y1" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="Z1" s="9" t="s">
+      <c r="Z1" s="10" t="s">
         <v>163</v>
       </c>
-      <c r="AA1" s="9" t="s">
+      <c r="AA1" s="10" t="s">
         <v>164</v>
       </c>
-      <c r="AB1" s="9" t="s">
+      <c r="AB1" s="10" t="s">
         <v>165</v>
       </c>
-      <c r="AC1" s="9" t="s">
+      <c r="AC1" s="10" t="s">
         <v>166</v>
       </c>
-      <c r="AD1" s="9" t="s">
+      <c r="AD1" s="10" t="s">
         <v>167</v>
       </c>
-      <c r="AE1" s="8" t="s">
+      <c r="AE1" s="9" t="s">
         <v>168</v>
       </c>
-      <c r="AF1" s="8" t="s">
+      <c r="AF1" s="9" t="s">
         <v>169</v>
       </c>
-      <c r="AG1" s="3" t="s">
+      <c r="AG1" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="AH1" s="6" t="s">
+      <c r="AH1" s="7" t="s">
         <v>171</v>
       </c>
-      <c r="AI1" s="8" t="s">
+      <c r="AI1" s="9" t="s">
         <v>172</v>
       </c>
-      <c r="AJ1" s="3" t="s">
+      <c r="AJ1" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="AK1" s="8" t="s">
+      <c r="AK1" s="9" t="s">
         <v>174</v>
       </c>
-      <c r="AL1" s="8" t="s">
+      <c r="AL1" s="9" t="s">
         <v>175</v>
       </c>
-      <c r="AM1" s="3" t="s">
+      <c r="AM1" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="AN1" s="8" t="s">
+      <c r="AN1" s="9" t="s">
         <v>177</v>
       </c>
-      <c r="AO1" s="8" t="s">
+      <c r="AO1" s="9" t="s">
         <v>178</v>
       </c>
-      <c r="AP1" s="3" t="s">
+      <c r="AP1" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="AQ1" s="3" t="s">
+      <c r="AQ1" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="AR1" s="3" t="s">
+      <c r="AR1" s="4" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="2" s="3" customFormat="1" ht="15" spans="1:44">
-      <c r="A2" s="5" t="s">
+    <row r="2" s="4" customFormat="1" ht="15" spans="1:44">
+      <c r="A2" s="6" t="s">
         <v>182</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="16" t="s">
         <v>183</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="4" t="s">
         <v>184</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="4" t="s">
         <v>185</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="K2" s="7" t="s">
+      <c r="K2" s="8" t="s">
         <v>187</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="L2" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="M2" s="5" t="s">
+      <c r="M2" s="6" t="s">
         <v>189</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="N2" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="O2" s="5" t="s">
+      <c r="O2" s="6" t="s">
         <v>190</v>
       </c>
-      <c r="P2" s="5" t="s">
+      <c r="P2" s="6" t="s">
         <v>191</v>
       </c>
-      <c r="Q2" s="3" t="s">
+      <c r="Q2" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="R2" s="5" t="s">
+      <c r="R2" s="6" t="s">
         <v>193</v>
       </c>
-      <c r="S2" s="3" t="s">
+      <c r="S2" s="4" t="s">
         <v>194</v>
       </c>
-      <c r="T2" s="15" t="s">
+      <c r="T2" s="16" t="s">
         <v>195</v>
       </c>
-      <c r="U2" s="3">
+      <c r="U2" s="4">
         <v>12500.45</v>
       </c>
-      <c r="V2" s="15" t="s">
+      <c r="V2" s="16" t="s">
         <v>196</v>
       </c>
-      <c r="W2" s="3" t="s">
+      <c r="W2" s="4" t="s">
         <v>197</v>
       </c>
-      <c r="X2" s="3" t="s">
+      <c r="X2" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="Y2" s="5" t="s">
+      <c r="Y2" s="6" t="s">
         <v>199</v>
       </c>
-      <c r="Z2" s="5" t="s">
+      <c r="Z2" s="6" t="s">
         <v>200</v>
       </c>
-      <c r="AA2" s="5" t="s">
+      <c r="AA2" s="6" t="s">
         <v>201</v>
       </c>
-      <c r="AB2" s="15" t="s">
+      <c r="AB2" s="16" t="s">
         <v>202</v>
       </c>
-      <c r="AC2" s="15" t="s">
+      <c r="AC2" s="16" t="s">
         <v>203</v>
       </c>
-      <c r="AL2" s="15" t="s">
+      <c r="AL2" s="16" t="s">
         <v>204</v>
       </c>
-      <c r="AM2" s="15" t="s">
+      <c r="AM2" s="16" t="s">
         <v>205</v>
       </c>
-      <c r="AQ2" s="10" t="s">
+      <c r="AQ2" s="11" t="s">
         <v>206</v>
       </c>
-      <c r="AR2" s="11" t="s">
+      <c r="AR2" s="12" t="s">
         <v>207</v>
       </c>
     </row>
@@ -2787,619 +2796,619 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="6"/>
   <sheetData>
-    <row r="1" s="3" customFormat="1" ht="38.25" spans="1:44">
-      <c r="A1" s="3" t="s">
+    <row r="1" s="4" customFormat="1" ht="38.25" spans="1:44">
+      <c r="A1" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="L1" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="M1" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="N1" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="O1" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="P1" s="7" t="s">
         <v>153</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="Q1" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="R1" s="6" t="s">
+      <c r="R1" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="S1" s="6" t="s">
+      <c r="S1" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="T1" s="6" t="s">
+      <c r="T1" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="U1" s="6" t="s">
+      <c r="U1" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="V1" s="6" t="s">
+      <c r="V1" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="W1" s="6" t="s">
+      <c r="W1" s="7" t="s">
         <v>160</v>
       </c>
-      <c r="X1" s="6" t="s">
+      <c r="X1" s="7" t="s">
         <v>161</v>
       </c>
-      <c r="Y1" s="8" t="s">
+      <c r="Y1" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="Z1" s="9" t="s">
+      <c r="Z1" s="10" t="s">
         <v>163</v>
       </c>
-      <c r="AA1" s="9" t="s">
+      <c r="AA1" s="10" t="s">
         <v>164</v>
       </c>
-      <c r="AB1" s="9" t="s">
+      <c r="AB1" s="10" t="s">
         <v>165</v>
       </c>
-      <c r="AC1" s="9" t="s">
+      <c r="AC1" s="10" t="s">
         <v>166</v>
       </c>
-      <c r="AD1" s="9" t="s">
+      <c r="AD1" s="10" t="s">
         <v>167</v>
       </c>
-      <c r="AE1" s="8" t="s">
+      <c r="AE1" s="9" t="s">
         <v>168</v>
       </c>
-      <c r="AF1" s="8" t="s">
+      <c r="AF1" s="9" t="s">
         <v>169</v>
       </c>
-      <c r="AG1" s="3" t="s">
+      <c r="AG1" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="AH1" s="6" t="s">
+      <c r="AH1" s="7" t="s">
         <v>171</v>
       </c>
-      <c r="AI1" s="8" t="s">
+      <c r="AI1" s="9" t="s">
         <v>172</v>
       </c>
-      <c r="AJ1" s="3" t="s">
+      <c r="AJ1" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="AK1" s="8" t="s">
+      <c r="AK1" s="9" t="s">
         <v>174</v>
       </c>
-      <c r="AL1" s="8" t="s">
+      <c r="AL1" s="9" t="s">
         <v>175</v>
       </c>
-      <c r="AM1" s="3" t="s">
+      <c r="AM1" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="AN1" s="8" t="s">
+      <c r="AN1" s="9" t="s">
         <v>177</v>
       </c>
-      <c r="AO1" s="8" t="s">
+      <c r="AO1" s="9" t="s">
         <v>178</v>
       </c>
-      <c r="AP1" s="3" t="s">
+      <c r="AP1" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="AQ1" s="3" t="s">
+      <c r="AQ1" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="AR1" s="3" t="s">
+      <c r="AR1" s="4" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="2" s="3" customFormat="1" ht="45" spans="1:44">
-      <c r="A2" s="5" t="s">
+    <row r="2" s="4" customFormat="1" ht="45" spans="1:44">
+      <c r="A2" s="6" t="s">
         <v>182</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="16" t="s">
         <v>183</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="4" t="s">
         <v>184</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="4" t="s">
         <v>208</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="J2" s="15" t="s">
+      <c r="J2" s="16" t="s">
         <v>210</v>
       </c>
-      <c r="K2" s="12" t="s">
+      <c r="K2" s="13" t="s">
         <v>211</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="L2" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="M2" s="5" t="s">
+      <c r="M2" s="6" t="s">
         <v>189</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="N2" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="O2" s="5" t="s">
+      <c r="O2" s="6" t="s">
         <v>190</v>
       </c>
-      <c r="P2" s="5" t="s">
+      <c r="P2" s="6" t="s">
         <v>191</v>
       </c>
-      <c r="Q2" s="3" t="s">
+      <c r="Q2" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="R2" s="5" t="s">
+      <c r="R2" s="6" t="s">
         <v>193</v>
       </c>
-      <c r="S2" s="3" t="s">
+      <c r="S2" s="4" t="s">
         <v>194</v>
       </c>
-      <c r="T2" s="15" t="s">
+      <c r="T2" s="16" t="s">
         <v>195</v>
       </c>
-      <c r="U2" s="15" t="s">
+      <c r="U2" s="16" t="s">
         <v>212</v>
       </c>
-      <c r="V2" s="15" t="s">
+      <c r="V2" s="16" t="s">
         <v>213</v>
       </c>
-      <c r="W2" s="3" t="s">
+      <c r="W2" s="4" t="s">
         <v>197</v>
       </c>
-      <c r="X2" s="3" t="s">
+      <c r="X2" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="Y2" s="5" t="s">
+      <c r="Y2" s="6" t="s">
         <v>199</v>
       </c>
-      <c r="Z2" s="5" t="s">
+      <c r="Z2" s="6" t="s">
         <v>200</v>
       </c>
-      <c r="AA2" s="5" t="s">
+      <c r="AA2" s="6" t="s">
         <v>201</v>
       </c>
-      <c r="AB2" s="3">
+      <c r="AB2" s="4">
         <v>14000</v>
       </c>
-      <c r="AC2" s="3">
+      <c r="AC2" s="4">
         <v>50000</v>
       </c>
-      <c r="AL2" s="15" t="s">
+      <c r="AL2" s="16" t="s">
         <v>204</v>
       </c>
-      <c r="AM2" s="15" t="s">
+      <c r="AM2" s="16" t="s">
         <v>205</v>
       </c>
-      <c r="AQ2" s="10" t="s">
+      <c r="AQ2" s="11" t="s">
         <v>214</v>
       </c>
-      <c r="AR2" s="14" t="s">
+      <c r="AR2" s="15" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="3" s="3" customFormat="1" spans="1:44">
-      <c r="A3" s="5" t="s">
+    <row r="3" s="4" customFormat="1" spans="1:44">
+      <c r="A3" s="6" t="s">
         <v>216</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="D3" s="16" t="s">
         <v>217</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="4" t="s">
         <v>184</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="6" t="s">
         <v>218</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="H3" s="4" t="s">
         <v>219</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="I3" s="4" t="s">
         <v>220</v>
       </c>
-      <c r="J3" s="15" t="s">
+      <c r="J3" s="16" t="s">
         <v>221</v>
       </c>
-      <c r="K3" s="10" t="s">
+      <c r="K3" s="11" t="s">
         <v>222</v>
       </c>
-      <c r="L3" s="5" t="s">
+      <c r="L3" s="6" t="s">
         <v>223</v>
       </c>
-      <c r="M3" s="5" t="s">
+      <c r="M3" s="6" t="s">
         <v>189</v>
       </c>
-      <c r="N3" s="3" t="s">
+      <c r="N3" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="O3" s="5" t="s">
+      <c r="O3" s="6" t="s">
         <v>224</v>
       </c>
-      <c r="P3" s="5" t="s">
+      <c r="P3" s="6" t="s">
         <v>225</v>
       </c>
-      <c r="Q3" s="3" t="s">
+      <c r="Q3" s="4" t="s">
         <v>226</v>
       </c>
-      <c r="R3" s="5" t="s">
+      <c r="R3" s="6" t="s">
         <v>227</v>
       </c>
-      <c r="S3" s="3" t="s">
+      <c r="S3" s="4" t="s">
         <v>197</v>
       </c>
-      <c r="T3" s="15" t="s">
+      <c r="T3" s="16" t="s">
         <v>228</v>
       </c>
-      <c r="U3" s="15" t="s">
+      <c r="U3" s="16" t="s">
         <v>213</v>
       </c>
-      <c r="V3" s="15" t="s">
+      <c r="V3" s="16" t="s">
         <v>229</v>
       </c>
-      <c r="W3" s="3" t="s">
+      <c r="W3" s="4" t="s">
         <v>194</v>
       </c>
-      <c r="X3" s="5" t="s">
+      <c r="X3" s="6" t="s">
         <v>230</v>
       </c>
-      <c r="Y3" s="5" t="s">
+      <c r="Y3" s="6" t="s">
         <v>231</v>
       </c>
-      <c r="Z3" s="5" t="s">
+      <c r="Z3" s="6" t="s">
         <v>232</v>
       </c>
-      <c r="AA3" s="5" t="s">
+      <c r="AA3" s="6" t="s">
         <v>233</v>
       </c>
-      <c r="AB3" s="3">
+      <c r="AB3" s="4">
         <v>25000</v>
       </c>
-      <c r="AC3" s="3">
+      <c r="AC3" s="4">
         <v>10000</v>
       </c>
-      <c r="AL3" s="15" t="s">
+      <c r="AL3" s="16" t="s">
         <v>234</v>
       </c>
-      <c r="AM3" s="15" t="s">
+      <c r="AM3" s="16" t="s">
         <v>235</v>
       </c>
-      <c r="AQ3" s="10" t="s">
+      <c r="AQ3" s="11" t="s">
         <v>206</v>
       </c>
-      <c r="AR3" s="14" t="s">
+      <c r="AR3" s="15" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="5" s="3" customFormat="1" ht="45" spans="1:44">
-      <c r="A5" s="5" t="s">
+    <row r="5" s="4" customFormat="1" ht="45" spans="1:44">
+      <c r="A5" s="6" t="s">
         <v>182</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="D5" s="15" t="s">
+      <c r="D5" s="16" t="s">
         <v>183</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="4" t="s">
         <v>184</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="H5" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="I5" s="3" t="s">
+      <c r="I5" s="4" t="s">
         <v>238</v>
       </c>
-      <c r="J5" s="15" t="s">
+      <c r="J5" s="16" t="s">
         <v>210</v>
       </c>
-      <c r="K5" s="12" t="s">
+      <c r="K5" s="13" t="s">
         <v>211</v>
       </c>
-      <c r="L5" s="3" t="s">
+      <c r="L5" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="M5" s="5" t="s">
+      <c r="M5" s="6" t="s">
         <v>189</v>
       </c>
-      <c r="N5" s="3" t="s">
+      <c r="N5" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="O5" s="5" t="s">
+      <c r="O5" s="6" t="s">
         <v>190</v>
       </c>
-      <c r="P5" s="5" t="s">
+      <c r="P5" s="6" t="s">
         <v>191</v>
       </c>
-      <c r="Q5" s="3" t="s">
+      <c r="Q5" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="R5" s="5" t="s">
+      <c r="R5" s="6" t="s">
         <v>193</v>
       </c>
-      <c r="S5" s="3" t="s">
+      <c r="S5" s="4" t="s">
         <v>194</v>
       </c>
-      <c r="T5" s="15" t="s">
+      <c r="T5" s="16" t="s">
         <v>195</v>
       </c>
-      <c r="U5" s="3">
+      <c r="U5" s="4">
         <v>12500.45</v>
       </c>
-      <c r="V5" s="3">
+      <c r="V5" s="4">
         <v>123456.789</v>
       </c>
-      <c r="W5" s="3" t="s">
+      <c r="W5" s="4" t="s">
         <v>197</v>
       </c>
-      <c r="X5" s="3" t="s">
+      <c r="X5" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="Y5" s="5" t="s">
+      <c r="Y5" s="6" t="s">
         <v>199</v>
       </c>
-      <c r="Z5" s="5" t="s">
+      <c r="Z5" s="6" t="s">
         <v>200</v>
       </c>
-      <c r="AA5" s="5" t="s">
+      <c r="AA5" s="6" t="s">
         <v>201</v>
       </c>
-      <c r="AB5" s="3">
+      <c r="AB5" s="4">
         <v>15800.56</v>
       </c>
-      <c r="AC5" s="3">
+      <c r="AC5" s="4">
         <v>50000.48</v>
       </c>
-      <c r="AL5" s="15" t="s">
+      <c r="AL5" s="16" t="s">
         <v>204</v>
       </c>
-      <c r="AM5" s="15" t="s">
+      <c r="AM5" s="16" t="s">
         <v>205</v>
       </c>
-      <c r="AQ5" s="10" t="s">
+      <c r="AQ5" s="11" t="s">
         <v>214</v>
       </c>
-      <c r="AR5" s="14" t="s">
+      <c r="AR5" s="15" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="6" s="3" customFormat="1" spans="1:44">
-      <c r="A6" s="5" t="s">
+    <row r="6" s="4" customFormat="1" spans="1:44">
+      <c r="A6" s="6" t="s">
         <v>216</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="D6" s="15" t="s">
+      <c r="D6" s="16" t="s">
         <v>217</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="4" t="s">
         <v>184</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="6" t="s">
         <v>218</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="H6" s="4" t="s">
         <v>240</v>
       </c>
-      <c r="I6" s="3" t="s">
+      <c r="I6" s="4" t="s">
         <v>241</v>
       </c>
-      <c r="J6" s="3">
+      <c r="J6" s="4">
         <v>1234567890</v>
       </c>
-      <c r="K6" s="10" t="s">
+      <c r="K6" s="11" t="s">
         <v>222</v>
       </c>
-      <c r="L6" s="5" t="s">
+      <c r="L6" s="6" t="s">
         <v>223</v>
       </c>
-      <c r="M6" s="5" t="s">
+      <c r="M6" s="6" t="s">
         <v>189</v>
       </c>
-      <c r="N6" s="3" t="s">
+      <c r="N6" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="O6" s="5" t="s">
+      <c r="O6" s="6" t="s">
         <v>224</v>
       </c>
-      <c r="P6" s="5" t="s">
+      <c r="P6" s="6" t="s">
         <v>225</v>
       </c>
-      <c r="Q6" s="3" t="s">
+      <c r="Q6" s="4" t="s">
         <v>226</v>
       </c>
-      <c r="R6" s="5" t="s">
+      <c r="R6" s="6" t="s">
         <v>227</v>
       </c>
-      <c r="S6" s="3" t="s">
+      <c r="S6" s="4" t="s">
         <v>197</v>
       </c>
-      <c r="T6" s="13">
+      <c r="T6" s="14">
         <v>43133</v>
       </c>
-      <c r="V6" s="15" t="s">
+      <c r="V6" s="16" t="s">
         <v>242</v>
       </c>
-      <c r="W6" s="3" t="s">
+      <c r="W6" s="4" t="s">
         <v>194</v>
       </c>
-      <c r="X6" s="5" t="s">
+      <c r="X6" s="6" t="s">
         <v>230</v>
       </c>
-      <c r="Y6" s="5" t="s">
+      <c r="Y6" s="6" t="s">
         <v>231</v>
       </c>
-      <c r="Z6" s="5" t="s">
+      <c r="Z6" s="6" t="s">
         <v>232</v>
       </c>
-      <c r="AA6" s="5" t="s">
+      <c r="AA6" s="6" t="s">
         <v>233</v>
       </c>
-      <c r="AB6" s="3">
+      <c r="AB6" s="4">
         <v>25000</v>
       </c>
-      <c r="AL6" s="15" t="s">
+      <c r="AL6" s="16" t="s">
         <v>234</v>
       </c>
-      <c r="AM6" s="15" t="s">
+      <c r="AM6" s="16" t="s">
         <v>235</v>
       </c>
-      <c r="AQ6" s="10" t="s">
+      <c r="AQ6" s="11" t="s">
         <v>206</v>
       </c>
-      <c r="AR6" s="14" t="s">
+      <c r="AR6" s="15" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="7" s="3" customFormat="1" spans="1:44">
-      <c r="A7" s="5" t="s">
+    <row r="7" s="4" customFormat="1" spans="1:44">
+      <c r="A7" s="6" t="s">
         <v>216</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="3" t="s">
         <v>244</v>
       </c>
-      <c r="C7" s="5"/>
-      <c r="D7" s="3" t="s">
+      <c r="C7" s="6"/>
+      <c r="D7" s="4" t="s">
         <v>217</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="4" t="s">
         <v>184</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="F7" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="H7" s="4" t="s">
         <v>246</v>
       </c>
-      <c r="I7" s="3" t="s">
+      <c r="I7" s="4" t="s">
         <v>247</v>
       </c>
-      <c r="J7" s="3" t="s">
+      <c r="J7" s="4" t="s">
         <v>248</v>
       </c>
-      <c r="K7" s="10" t="s">
+      <c r="K7" s="11" t="s">
         <v>222</v>
       </c>
-      <c r="L7" s="5" t="s">
+      <c r="L7" s="6" t="s">
         <v>223</v>
       </c>
-      <c r="M7" s="5" t="s">
+      <c r="M7" s="6" t="s">
         <v>189</v>
       </c>
-      <c r="N7" s="3" t="s">
+      <c r="N7" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="O7" s="5" t="s">
+      <c r="O7" s="6" t="s">
         <v>224</v>
       </c>
-      <c r="P7" s="5" t="s">
+      <c r="P7" s="6" t="s">
         <v>225</v>
       </c>
-      <c r="Q7" s="3" t="s">
+      <c r="Q7" s="4" t="s">
         <v>226</v>
       </c>
-      <c r="R7" s="5" t="s">
+      <c r="R7" s="6" t="s">
         <v>227</v>
       </c>
-      <c r="S7" s="3" t="s">
+      <c r="S7" s="4" t="s">
         <v>197</v>
       </c>
-      <c r="T7" s="13">
+      <c r="T7" s="14">
         <v>43133</v>
       </c>
-      <c r="U7" s="3">
+      <c r="U7" s="4">
         <v>0</v>
       </c>
-      <c r="V7" s="3" t="s">
+      <c r="V7" s="4" t="s">
         <v>249</v>
       </c>
-      <c r="W7" s="3" t="s">
+      <c r="W7" s="4" t="s">
         <v>194</v>
       </c>
-      <c r="X7" s="5" t="s">
+      <c r="X7" s="6" t="s">
         <v>230</v>
       </c>
-      <c r="Y7" s="5" t="s">
+      <c r="Y7" s="6" t="s">
         <v>231</v>
       </c>
-      <c r="Z7" s="5" t="s">
+      <c r="Z7" s="6" t="s">
         <v>232</v>
       </c>
-      <c r="AA7" s="5" t="s">
+      <c r="AA7" s="6" t="s">
         <v>233</v>
       </c>
-      <c r="AB7" s="3">
+      <c r="AB7" s="4">
         <v>25000.88</v>
       </c>
-      <c r="AC7" s="3">
+      <c r="AC7" s="4">
         <v>0</v>
       </c>
-      <c r="AL7" s="3" t="s">
+      <c r="AL7" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="AM7" s="3" t="s">
+      <c r="AM7" s="4" t="s">
         <v>235</v>
       </c>
-      <c r="AQ7" s="10" t="s">
+      <c r="AQ7" s="11" t="s">
         <v>206</v>
       </c>
-      <c r="AR7" s="14" t="s">
+      <c r="AR7" s="15" t="s">
         <v>250</v>
       </c>
     </row>
@@ -3432,217 +3441,217 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75" outlineLevelRow="1"/>
   <cols>
-    <col min="1" max="1" width="9.14285714285714" style="3"/>
-    <col min="2" max="2" width="28.7142857142857" style="3" customWidth="1"/>
-    <col min="3" max="3" width="13.1428571428571" style="3" customWidth="1"/>
-    <col min="4" max="5" width="9.14285714285714" style="3"/>
-    <col min="6" max="6" width="28" style="3" customWidth="1"/>
-    <col min="7" max="9" width="9.14285714285714" style="3"/>
-    <col min="10" max="10" width="13.8571428571429" style="3" customWidth="1"/>
-    <col min="11" max="11" width="25.2857142857143" style="3" customWidth="1"/>
-    <col min="12" max="12" width="9.14285714285714" style="3"/>
-    <col min="13" max="13" width="14.5714285714286" style="3" customWidth="1"/>
-    <col min="14" max="14" width="9.14285714285714" style="3"/>
-    <col min="15" max="15" width="47.5714285714286" style="3" customWidth="1"/>
-    <col min="16" max="16" width="9.14285714285714" style="3"/>
-    <col min="17" max="17" width="12.2857142857143" style="3" customWidth="1"/>
-    <col min="18" max="18" width="20.7142857142857" style="3" customWidth="1"/>
-    <col min="19" max="19" width="9.14285714285714" style="3"/>
-    <col min="20" max="20" width="12" style="3" customWidth="1"/>
-    <col min="21" max="21" width="9.57142857142857" style="3"/>
-    <col min="22" max="22" width="11.7142857142857" style="3"/>
-    <col min="23" max="23" width="9.14285714285714" style="3"/>
-    <col min="24" max="24" width="23.2857142857143" style="3" customWidth="1"/>
-    <col min="25" max="25" width="34.5714285714286" style="3" customWidth="1"/>
-    <col min="26" max="26" width="23.7142857142857" style="3" customWidth="1"/>
-    <col min="27" max="27" width="43" style="3" customWidth="1"/>
-    <col min="28" max="29" width="9.14285714285714" style="3"/>
-    <col min="30" max="30" width="35.7142857142857" style="3" customWidth="1"/>
-    <col min="31" max="31" width="29.5714285714286" style="3" customWidth="1"/>
-    <col min="32" max="16384" width="9.14285714285714" style="3"/>
+    <col min="1" max="1" width="9.14285714285714" style="4"/>
+    <col min="2" max="2" width="28.7142857142857" style="4" customWidth="1"/>
+    <col min="3" max="3" width="13.1428571428571" style="4" customWidth="1"/>
+    <col min="4" max="5" width="9.14285714285714" style="4"/>
+    <col min="6" max="6" width="28" style="4" customWidth="1"/>
+    <col min="7" max="9" width="9.14285714285714" style="4"/>
+    <col min="10" max="10" width="13.8571428571429" style="4" customWidth="1"/>
+    <col min="11" max="11" width="25.2857142857143" style="4" customWidth="1"/>
+    <col min="12" max="12" width="9.14285714285714" style="4"/>
+    <col min="13" max="13" width="14.5714285714286" style="4" customWidth="1"/>
+    <col min="14" max="14" width="9.14285714285714" style="4"/>
+    <col min="15" max="15" width="47.5714285714286" style="4" customWidth="1"/>
+    <col min="16" max="16" width="9.14285714285714" style="4"/>
+    <col min="17" max="17" width="12.2857142857143" style="4" customWidth="1"/>
+    <col min="18" max="18" width="20.7142857142857" style="4" customWidth="1"/>
+    <col min="19" max="19" width="9.14285714285714" style="4"/>
+    <col min="20" max="20" width="12" style="4" customWidth="1"/>
+    <col min="21" max="21" width="9.57142857142857" style="4"/>
+    <col min="22" max="22" width="11.7142857142857" style="4"/>
+    <col min="23" max="23" width="9.14285714285714" style="4"/>
+    <col min="24" max="24" width="23.2857142857143" style="4" customWidth="1"/>
+    <col min="25" max="25" width="34.5714285714286" style="4" customWidth="1"/>
+    <col min="26" max="26" width="23.7142857142857" style="4" customWidth="1"/>
+    <col min="27" max="27" width="43" style="4" customWidth="1"/>
+    <col min="28" max="29" width="9.14285714285714" style="4"/>
+    <col min="30" max="30" width="35.7142857142857" style="4" customWidth="1"/>
+    <col min="31" max="31" width="29.5714285714286" style="4" customWidth="1"/>
+    <col min="32" max="16384" width="9.14285714285714" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" s="3" customFormat="1" ht="25.5" spans="1:31">
-      <c r="A1" s="3" t="s">
+    <row r="1" s="4" customFormat="1" ht="25.5" spans="1:31">
+      <c r="A1" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="L1" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="M1" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="N1" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="O1" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="P1" s="7" t="s">
         <v>153</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="Q1" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="R1" s="6" t="s">
+      <c r="R1" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="S1" s="6" t="s">
+      <c r="S1" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="T1" s="6" t="s">
+      <c r="T1" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="U1" s="6" t="s">
+      <c r="U1" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="V1" s="6" t="s">
+      <c r="V1" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="W1" s="6" t="s">
+      <c r="W1" s="7" t="s">
         <v>160</v>
       </c>
-      <c r="X1" s="6" t="s">
+      <c r="X1" s="7" t="s">
         <v>161</v>
       </c>
-      <c r="Y1" s="8" t="s">
+      <c r="Y1" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="Z1" s="9" t="s">
+      <c r="Z1" s="10" t="s">
         <v>163</v>
       </c>
-      <c r="AA1" s="9" t="s">
+      <c r="AA1" s="10" t="s">
         <v>164</v>
       </c>
-      <c r="AB1" s="8" t="s">
+      <c r="AB1" s="9" t="s">
         <v>175</v>
       </c>
-      <c r="AC1" s="3" t="s">
+      <c r="AC1" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="AD1" s="3" t="s">
+      <c r="AD1" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="AE1" s="3" t="s">
+      <c r="AE1" s="4" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="2" s="3" customFormat="1" ht="15" spans="1:31">
-      <c r="A2" s="5" t="s">
+    <row r="2" s="4" customFormat="1" ht="15" spans="1:31">
+      <c r="A2" s="6" t="s">
         <v>216</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="16" t="s">
         <v>183</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="4" t="s">
         <v>184</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="4" t="s">
         <v>251</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="4" t="s">
         <v>252</v>
       </c>
-      <c r="K2" s="7" t="s">
+      <c r="K2" s="8" t="s">
         <v>187</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="L2" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="M2" s="5" t="s">
+      <c r="M2" s="6" t="s">
         <v>189</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="N2" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="O2" s="5" t="s">
+      <c r="O2" s="6" t="s">
         <v>253</v>
       </c>
-      <c r="P2" s="5" t="s">
+      <c r="P2" s="6" t="s">
         <v>191</v>
       </c>
-      <c r="Q2" s="3" t="s">
+      <c r="Q2" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="R2" s="5" t="s">
+      <c r="R2" s="6" t="s">
         <v>193</v>
       </c>
-      <c r="S2" s="3" t="s">
+      <c r="S2" s="4" t="s">
         <v>194</v>
       </c>
-      <c r="T2" s="15" t="s">
+      <c r="T2" s="16" t="s">
         <v>195</v>
       </c>
-      <c r="U2" s="3">
+      <c r="U2" s="4">
         <v>12500.45</v>
       </c>
-      <c r="V2" s="15" t="s">
+      <c r="V2" s="16" t="s">
         <v>196</v>
       </c>
-      <c r="W2" s="3" t="s">
+      <c r="W2" s="4" t="s">
         <v>197</v>
       </c>
-      <c r="X2" s="3" t="s">
+      <c r="X2" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="Y2" s="5" t="s">
+      <c r="Y2" s="6" t="s">
         <v>199</v>
       </c>
-      <c r="Z2" s="5" t="s">
+      <c r="Z2" s="6" t="s">
         <v>200</v>
       </c>
-      <c r="AA2" s="5" t="s">
+      <c r="AA2" s="6" t="s">
         <v>201</v>
       </c>
-      <c r="AB2" s="3">
+      <c r="AB2" s="4">
         <v>10</v>
       </c>
-      <c r="AC2" s="3">
+      <c r="AC2" s="4">
         <v>17</v>
       </c>
-      <c r="AD2" s="10" t="s">
+      <c r="AD2" s="11" t="s">
         <v>206</v>
       </c>
-      <c r="AE2" s="11" t="s">
+      <c r="AE2" s="12" t="s">
         <v>207</v>
       </c>
     </row>
@@ -3825,7 +3834,7 @@
       <c r="J2">
         <v>9830123456</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="K2" s="2" t="s">
         <v>264</v>
       </c>
       <c r="L2" t="s">
@@ -3837,7 +3846,7 @@
       <c r="N2" t="s">
         <v>100</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="O2" s="3" t="s">
         <v>224</v>
       </c>
       <c r="P2" t="s">
@@ -3905,4 +3914,47 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="5"/>
+  <cols>
+    <col min="1" max="1" width="18" customWidth="1"/>
+    <col min="2" max="2" width="16.4285714285714" customWidth="1"/>
+    <col min="3" max="3" width="20" customWidth="1"/>
+    <col min="4" max="4" width="17.8571428571429" customWidth="1"/>
+    <col min="5" max="5" width="14.4285714285714" customWidth="1"/>
+    <col min="6" max="6" width="12.7142857142857" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="F1" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>